<commit_message>
Updated database.  Added override table
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
   <si>
     <t>Model</t>
   </si>
@@ -24,19 +24,7 @@
     <t>ModelNum</t>
   </si>
   <si>
-    <t>RouteNum</t>
-  </si>
-  <si>
     <t>TotalTime</t>
-  </si>
-  <si>
-    <t>IsOverrideActive</t>
-  </si>
-  <si>
-    <t>OverrideRoute</t>
-  </si>
-  <si>
-    <t>OverrideTime</t>
   </si>
   <si>
     <t>BoxSize</t>
@@ -542,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,453 +541,333 @@
     <col min="1" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>8001</v>
+      </c>
+      <c r="J3">
+        <v>150000</v>
+      </c>
+      <c r="K3" s="8">
+        <v>43252</v>
+      </c>
+      <c r="L3">
+        <f>M3+N3+P14+P15+P16+P17</f>
+        <v>6.35</v>
+      </c>
+      <c r="M3">
+        <v>2.25</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>8001</v>
-      </c>
-      <c r="O3">
-        <v>150000</v>
-      </c>
-      <c r="P3" s="8">
-        <v>43252</v>
-      </c>
-      <c r="Q3">
-        <f>R3+S3+P14+P15+P16+P17</f>
-        <v>6.35</v>
-      </c>
-      <c r="R3">
-        <v>2.25</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
+      <c r="D4">
+        <v>1.5</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
+        <v>8002</v>
+      </c>
+      <c r="J4">
+        <v>150000</v>
+      </c>
+      <c r="K4" s="8">
+        <v>43253</v>
+      </c>
+      <c r="L4">
+        <f>M4+N4+P18+P19+P20+P21</f>
+        <v>6.2500000000000009</v>
+      </c>
+      <c r="M4">
+        <v>2.1</v>
+      </c>
+      <c r="N4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>1.5</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>8002</v>
-      </c>
-      <c r="O4">
-        <v>150000</v>
-      </c>
-      <c r="P4" s="8">
-        <v>43253</v>
-      </c>
-      <c r="Q4">
-        <f>R4+S4+P18+P19+P20+P21</f>
-        <v>6.2500000000000009</v>
-      </c>
-      <c r="R4">
-        <v>2.1</v>
-      </c>
-      <c r="S4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
       <c r="I5">
-        <v>2</v>
+        <v>8003</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>150000</v>
+      </c>
+      <c r="K5" s="8">
+        <v>43254</v>
+      </c>
+      <c r="L5">
+        <f>M5+N5</f>
+        <v>2.9</v>
+      </c>
+      <c r="M5">
+        <v>1.9</v>
       </c>
       <c r="N5">
-        <v>8003</v>
-      </c>
-      <c r="O5">
-        <v>150000</v>
-      </c>
-      <c r="P5" s="8">
-        <v>43254</v>
-      </c>
-      <c r="Q5">
-        <f>R5+S5</f>
-        <v>2.9</v>
-      </c>
-      <c r="R5">
-        <v>1.9</v>
-      </c>
-      <c r="S5">
         <v>1</v>
       </c>
-      <c r="T5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6">
+      <c r="I6">
+        <v>9001</v>
+      </c>
+      <c r="J6">
+        <v>151000</v>
+      </c>
+      <c r="K6" s="8">
+        <v>43255</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L7" si="0">M6+N6</f>
+        <v>3.85</v>
+      </c>
+      <c r="M6">
+        <v>2.1</v>
+      </c>
+      <c r="N6">
+        <v>1.75</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>9001</v>
-      </c>
-      <c r="O6">
-        <v>151000</v>
-      </c>
-      <c r="P6" s="8">
-        <v>43255</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" ref="Q6:Q7" si="0">R6+S6</f>
-        <v>3.85</v>
-      </c>
-      <c r="R6">
-        <v>2.1</v>
-      </c>
-      <c r="S6">
-        <v>1.75</v>
-      </c>
-      <c r="T6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
+      <c r="D7">
+        <v>1.5</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
       <c r="I7">
-        <v>1.5</v>
+        <v>9002</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>9002</v>
-      </c>
-      <c r="O7">
         <v>151000</v>
       </c>
-      <c r="P7" s="8">
+      <c r="K7" s="8">
         <v>43256</v>
       </c>
-      <c r="Q7">
+      <c r="L7">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="R7">
+      <c r="M7">
         <v>2.1</v>
       </c>
-      <c r="S7">
+      <c r="N7">
         <v>1.5</v>
       </c>
-      <c r="T7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
+      <c r="D9">
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9">
-        <v>4</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3">
         <v>0.5</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O14" s="7">
         <v>8001</v>
@@ -1008,24 +876,24 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
         <v>1.2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O15" s="7">
         <v>8001</v>
@@ -1034,24 +902,24 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3">
         <v>1.6</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O16" s="7">
         <v>8001</v>
@@ -1062,22 +930,22 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3">
         <v>0.6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O17" s="7">
         <v>8001</v>
@@ -1088,22 +956,22 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3">
         <v>0.75</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O18" s="6">
         <v>8002</v>
@@ -1114,22 +982,22 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O19" s="6">
         <v>8002</v>
@@ -1140,22 +1008,22 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" s="5">
         <v>0.75</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O20" s="6">
         <v>8002</v>
@@ -1166,22 +1034,22 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D21" s="5">
         <v>1.35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O21" s="6">
         <v>8002</v>
@@ -1192,74 +1060,75 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D22" s="5">
         <v>2</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D24" s="5">
         <v>1.25</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D25" s="5">
         <v>1.6</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1270,6 +1139,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added override function to home view
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>Model</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Override</t>
+  </si>
+  <si>
+    <t>IsOverrideActive</t>
+  </si>
+  <si>
+    <t>OverrideRoute</t>
+  </si>
+  <si>
+    <t>OverrideTime</t>
+  </si>
+  <si>
+    <t>Model_Base</t>
+  </si>
+  <si>
+    <t>A1C1A042PAB</t>
+  </si>
+  <si>
+    <t>A1C3B021PA</t>
   </si>
 </sst>
 </file>
@@ -219,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -229,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,18 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +569,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -587,7 +607,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -613,7 +633,7 @@
         <v>43252</v>
       </c>
       <c r="L3">
-        <f>M3+N3+P14+P15+P16+P17</f>
+        <f>M3+N3+K14+K15+K16+K17</f>
         <v>6.35</v>
       </c>
       <c r="M3">
@@ -626,7 +646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -652,7 +672,7 @@
         <v>43253</v>
       </c>
       <c r="L4">
-        <f>M4+N4+P18+P19+P20+P21</f>
+        <f>M4+N4+K18+K19+K20+K21</f>
         <v>6.2500000000000009</v>
       </c>
       <c r="M4">
@@ -665,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -704,7 +724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -743,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -782,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -799,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -816,314 +836,387 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="N12" t="s">
+      <c r="J12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" t="s">
-        <v>40</v>
-      </c>
-      <c r="P13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="7">
+      <c r="J14" s="7">
         <v>8001</v>
       </c>
-      <c r="P14" s="7">
+      <c r="K14" s="7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="I15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="7">
+        <v>8001</v>
+      </c>
+      <c r="K15" s="7">
         <v>1.2</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="7">
-        <v>8001</v>
-      </c>
-      <c r="P15" s="7">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="7">
+      <c r="J16" s="7">
         <v>8001</v>
       </c>
-      <c r="P16" s="7">
+      <c r="K16" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="7">
+      <c r="J17" s="7">
         <v>8001</v>
       </c>
-      <c r="P17" s="7">
+      <c r="K17" s="7">
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="6">
+      <c r="J18" s="6">
         <v>8002</v>
       </c>
-      <c r="P18" s="6">
+      <c r="K18" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="6">
+      <c r="J19" s="6">
         <v>8002</v>
       </c>
-      <c r="P19" s="6">
+      <c r="K19" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N20" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="6">
+      <c r="J20" s="6">
         <v>8002</v>
       </c>
-      <c r="P20" s="6">
+      <c r="K20" s="6">
         <v>0.65</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.35</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O21" s="6">
+      <c r="J21" s="6">
         <v>8002</v>
       </c>
-      <c r="P21" s="6">
+      <c r="K21" s="6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>38</v>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>2424</v>
+      </c>
+      <c r="D30">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>4848</v>
+      </c>
+      <c r="D31">
+        <v>48.6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>111222</v>
+      </c>
+      <c r="D32">
+        <v>28.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added filterable model and option tables
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -30,9 +30,6 @@
     <t>BoxSize</t>
   </si>
   <si>
-    <t>BaseTime</t>
-  </si>
-  <si>
     <t>AVTime</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>SalesOrder</t>
   </si>
   <si>
-    <t>Model_Model</t>
-  </si>
-  <si>
     <t>TimeTrialsOptionTime</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>A1C3B021PA</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>DriveTime</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -251,6 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,53 +567,53 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -643,15 +644,15 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -682,15 +683,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="O4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -721,15 +722,15 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -760,15 +761,15 @@
         <v>1.75</v>
       </c>
       <c r="O6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -799,15 +800,15 @@
         <v>1.5</v>
       </c>
       <c r="O7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -821,10 +822,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -838,56 +839,56 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3">
         <v>0.5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" s="7">
         <v>8001</v>
@@ -898,22 +899,22 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3">
         <v>1.2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="7">
         <v>8001</v>
@@ -924,22 +925,22 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="3">
         <v>1.6</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="7">
         <v>8001</v>
@@ -950,22 +951,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3">
         <v>0.6</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J17" s="7">
         <v>8001</v>
@@ -976,22 +977,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3">
         <v>0.75</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J18" s="6">
         <v>8002</v>
@@ -1002,22 +1003,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J19" s="6">
         <v>8002</v>
@@ -1028,22 +1029,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5">
         <v>0.75</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J20" s="6">
         <v>8002</v>
@@ -1054,22 +1055,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5">
         <v>1.35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J21" s="6">
         <v>8002</v>
@@ -1080,97 +1081,97 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="5">
         <v>2</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="5">
         <v>1.25</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="5">
         <v>1.6</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -1182,12 +1183,12 @@
         <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1199,12 +1200,12 @@
         <v>48.6</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -1216,7 +1217,7 @@
         <v>28.5</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of day.  Worked on Time Trial table for supervisor view
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="11325"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,24 +553,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="10.7109375" customWidth="1"/>
+    <col min="1" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -586,29 +586,29 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -624,30 +624,30 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="G3">
         <v>8001</v>
       </c>
+      <c r="H3">
+        <v>150000</v>
+      </c>
+      <c r="I3" s="8">
+        <v>43252</v>
+      </c>
       <c r="J3">
-        <v>150000</v>
-      </c>
-      <c r="K3" s="8">
-        <v>43252</v>
+        <f>K3+L3+I14+I15+I16+I17</f>
+        <v>6.35</v>
+      </c>
+      <c r="K3">
+        <v>2.25</v>
       </c>
       <c r="L3">
-        <f>M3+N3+K14+K15+K16+K17</f>
-        <v>6.35</v>
-      </c>
-      <c r="M3">
-        <v>2.25</v>
-      </c>
-      <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="M3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -663,30 +663,30 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="G4">
         <v>8002</v>
       </c>
+      <c r="H4">
+        <v>150000</v>
+      </c>
+      <c r="I4" s="8">
+        <v>43253</v>
+      </c>
       <c r="J4">
-        <v>150000</v>
-      </c>
-      <c r="K4" s="8">
-        <v>43253</v>
+        <f>K4+L4+I18+I19+I20+I21</f>
+        <v>6.2500000000000009</v>
+      </c>
+      <c r="K4">
+        <v>2.1</v>
       </c>
       <c r="L4">
-        <f>M4+N4+K18+K19+K20+K21</f>
-        <v>6.2500000000000009</v>
-      </c>
-      <c r="M4">
-        <v>2.1</v>
-      </c>
-      <c r="N4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O4" t="s">
+      <c r="M4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -702,30 +702,30 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="G5">
         <v>8003</v>
       </c>
+      <c r="H5">
+        <v>150000</v>
+      </c>
+      <c r="I5" s="8">
+        <v>43254</v>
+      </c>
       <c r="J5">
-        <v>150000</v>
-      </c>
-      <c r="K5" s="8">
-        <v>43254</v>
+        <f>K5+L5</f>
+        <v>2.9</v>
+      </c>
+      <c r="K5">
+        <v>1.9</v>
       </c>
       <c r="L5">
-        <f>M5+N5</f>
-        <v>2.9</v>
-      </c>
-      <c r="M5">
-        <v>1.9</v>
-      </c>
-      <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
+      <c r="M5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -741,30 +741,30 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="G6">
         <v>9001</v>
       </c>
+      <c r="H6">
+        <v>151000</v>
+      </c>
+      <c r="I6" s="8">
+        <v>43255</v>
+      </c>
       <c r="J6">
-        <v>151000</v>
-      </c>
-      <c r="K6" s="8">
-        <v>43255</v>
+        <f t="shared" ref="J6:J7" si="0">K6+L6</f>
+        <v>3.85</v>
+      </c>
+      <c r="K6">
+        <v>2.1</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L7" si="0">M6+N6</f>
-        <v>3.85</v>
-      </c>
-      <c r="M6">
-        <v>2.1</v>
-      </c>
-      <c r="N6">
         <v>1.75</v>
       </c>
-      <c r="O6" t="s">
+      <c r="M6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -780,30 +780,30 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="G7">
         <v>9002</v>
       </c>
+      <c r="H7">
+        <v>151000</v>
+      </c>
+      <c r="I7" s="8">
+        <v>43256</v>
+      </c>
       <c r="J7">
-        <v>151000</v>
-      </c>
-      <c r="K7" s="8">
-        <v>43256</v>
-      </c>
-      <c r="L7">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="M7">
+      <c r="K7">
         <v>2.1</v>
       </c>
-      <c r="N7">
+      <c r="L7">
         <v>1.5</v>
       </c>
-      <c r="O7" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -837,15 +837,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="I12" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -861,17 +861,17 @@
       <c r="E13" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -887,17 +887,17 @@
       <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="7">
+      <c r="H14" s="7">
         <v>8001</v>
       </c>
-      <c r="K14" s="7">
+      <c r="I14" s="7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -913,17 +913,17 @@
       <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="7">
+      <c r="H15" s="7">
         <v>8001</v>
       </c>
-      <c r="K15" s="7">
+      <c r="I15" s="7">
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -939,17 +939,17 @@
       <c r="E16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="7">
+      <c r="H16" s="7">
         <v>8001</v>
       </c>
-      <c r="K16" s="7">
+      <c r="I16" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -965,17 +965,17 @@
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="7">
+      <c r="H17" s="7">
         <v>8001</v>
       </c>
-      <c r="K17" s="7">
+      <c r="I17" s="7">
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -991,17 +991,17 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="6">
+      <c r="H18" s="6">
         <v>8002</v>
       </c>
-      <c r="K18" s="6">
+      <c r="I18" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1017,17 +1017,17 @@
       <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="6">
+      <c r="H19" s="6">
         <v>8002</v>
       </c>
-      <c r="K19" s="6">
+      <c r="I19" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1043,17 +1043,17 @@
       <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="6">
+      <c r="H20" s="6">
         <v>8002</v>
       </c>
-      <c r="K20" s="6">
+      <c r="I20" s="6">
         <v>0.65</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1069,17 +1069,17 @@
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="6">
+      <c r="H21" s="6">
         <v>8002</v>
       </c>
-      <c r="K21" s="6">
+      <c r="I21" s="6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -1147,12 +1147,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Added timeTrial table to supervisor view
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Model</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>DriveTime</t>
+  </si>
+  <si>
+    <t>NumOptions</t>
   </si>
 </sst>
 </file>
@@ -553,16 +556,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -605,10 +610,13 @@
         <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -643,11 +651,14 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -682,11 +693,14 @@
       <c r="L4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -721,11 +735,14 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -760,11 +777,14 @@
       <c r="L6">
         <v>1.75</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -799,11 +819,14 @@
       <c r="L7">
         <v>1.5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -820,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -837,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -845,7 +868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -871,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -897,7 +920,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -923,7 +946,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
end of day.  Worked on AddTimeTrialPopup
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22560" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,15 +559,15 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="10.7109375" customWidth="1"/>
+    <col min="1" max="8" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -610,13 +610,13 @@
         <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -651,14 +651,14 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -693,14 +693,14 @@
       <c r="L4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4">
         <v>4</v>
       </c>
-      <c r="N4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -735,14 +735,14 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="N5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -777,14 +777,14 @@
       <c r="L6">
         <v>1.75</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="N6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -819,14 +819,14 @@
       <c r="L7">
         <v>1.5</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7">
         <v>0</v>
       </c>
-      <c r="N7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -868,7 +868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -894,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -946,7 +946,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -972,7 +972,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -998,7 +998,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -1170,12 +1170,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1255,9 +1255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
@@ -1271,7 +1271,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Supervisor view and modified TimeTrial Model
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22560" windowHeight="8232"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>Model</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>NumOptions</t>
+  </si>
+  <si>
+    <t>OptionsText</t>
+  </si>
+  <si>
+    <t>PABTXY</t>
   </si>
 </sst>
 </file>
@@ -556,18 +562,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="10.6640625" customWidth="1"/>
+    <col min="1" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -615,8 +621,11 @@
       <c r="N2" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="O2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -657,8 +666,11 @@
       <c r="N3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -699,8 +711,11 @@
       <c r="N4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -742,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -784,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -826,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -843,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -860,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -868,7 +883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -894,7 +909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -920,7 +935,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -946,7 +961,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -972,7 +987,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -998,7 +1013,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1024,7 +1039,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1076,7 +1091,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1102,7 +1117,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -1153,7 +1168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -1170,12 +1185,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1209,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1226,7 +1241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1255,9 +1270,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
@@ -1271,7 +1286,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated AddTimeTrial and SupervisorView
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>Model</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>PABTXY</t>
+  </si>
+  <si>
+    <t>PATX</t>
+  </si>
+  <si>
+    <t>PBCTXZ</t>
   </si>
 </sst>
 </file>
@@ -562,11 +568,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -621,7 +625,7 @@
       <c r="N2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -651,7 +655,6 @@
         <v>43252</v>
       </c>
       <c r="J3">
-        <f>K3+L3+I14+I15+I16+I17</f>
         <v>6.35</v>
       </c>
       <c r="K3">
@@ -696,8 +699,7 @@
         <v>43253</v>
       </c>
       <c r="J4">
-        <f>K4+L4+I18+I19+I20+I21</f>
-        <v>6.2500000000000009</v>
+        <v>6.25</v>
       </c>
       <c r="K4">
         <v>2.1</v>
@@ -741,7 +743,6 @@
         <v>43254</v>
       </c>
       <c r="J5">
-        <f>K5+L5</f>
         <v>2.9</v>
       </c>
       <c r="K5">
@@ -774,29 +775,31 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>9001</v>
+        <v>8004</v>
       </c>
       <c r="H6">
-        <v>151000</v>
+        <v>150001</v>
       </c>
       <c r="I6" s="8">
-        <v>43255</v>
+        <v>43257</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J7" si="0">K6+L6</f>
-        <v>3.85</v>
+        <v>3.97</v>
       </c>
       <c r="K6">
-        <v>2.1</v>
+        <v>1.87</v>
       </c>
       <c r="L6">
-        <v>1.75</v>
+        <v>0.95</v>
       </c>
       <c r="M6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="O6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -816,32 +819,34 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>9002</v>
+        <v>8005</v>
       </c>
       <c r="H7">
-        <v>151000</v>
+        <v>150001</v>
       </c>
       <c r="I7" s="8">
-        <v>43256</v>
+        <v>43258</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>5.07</v>
       </c>
       <c r="K7">
-        <v>2.1</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="L7">
-        <v>1.5</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="M7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -855,6 +860,30 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>8006</v>
+      </c>
+      <c r="H8">
+        <v>150001</v>
+      </c>
+      <c r="I8" s="8">
+        <v>43258</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8">
         <v>0</v>
       </c>
     </row>
@@ -874,295 +903,340 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G9">
+        <v>8007</v>
+      </c>
+      <c r="H9">
+        <v>150002</v>
+      </c>
+      <c r="I9" s="8">
+        <v>43259</v>
+      </c>
+      <c r="J9">
+        <v>8.65</v>
+      </c>
+      <c r="K9">
+        <v>2.25</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>9001</v>
+      </c>
+      <c r="H10">
+        <v>151000</v>
+      </c>
+      <c r="I10" s="8">
+        <v>43255</v>
+      </c>
+      <c r="J10">
+        <v>3.85</v>
+      </c>
+      <c r="K10">
+        <v>2.1</v>
+      </c>
+      <c r="L10">
+        <v>1.75</v>
+      </c>
+      <c r="M10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>9002</v>
+      </c>
+      <c r="H11">
+        <v>151000</v>
+      </c>
+      <c r="I11" s="8">
+        <v>43256</v>
+      </c>
+      <c r="J11">
+        <v>3.6</v>
+      </c>
+      <c r="K11">
+        <v>2.1</v>
+      </c>
+      <c r="L11">
+        <v>1.5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="7">
-        <v>8001</v>
-      </c>
-      <c r="I14" s="7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="7">
-        <v>8001</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1.2</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3">
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H16" s="7">
         <v>8001</v>
       </c>
       <c r="I16" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H17" s="7">
         <v>8001</v>
       </c>
       <c r="I17" s="7">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3">
-        <v>0.75</v>
+        <v>1.6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="6">
-        <v>8002</v>
-      </c>
-      <c r="I18" s="6">
+      <c r="G18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="7">
+        <v>8001</v>
+      </c>
+      <c r="I18" s="7">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="6">
-        <v>8002</v>
-      </c>
-      <c r="I19" s="6">
-        <v>1.1000000000000001</v>
+      <c r="G19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="7">
+        <v>8001</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="H20" s="6">
         <v>8002</v>
       </c>
       <c r="I20" s="6">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="H21" s="6">
         <v>8002</v>
       </c>
       <c r="I21" s="6">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="5">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="G22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="6">
+        <v>8002</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>1.35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="G23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="6">
+        <v>8002</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="5">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>8</v>
@@ -1170,91 +1244,125 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="5">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>2424</v>
-      </c>
-      <c r="D30">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>4848</v>
-      </c>
-      <c r="D31">
-        <v>48.6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
       </c>
       <c r="C32">
+        <v>2424</v>
+      </c>
+      <c r="D32">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>4848</v>
+      </c>
+      <c r="D33">
+        <v>48.6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34">
         <v>111222</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>28.5</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E34" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Override Model Popup
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
   <si>
     <t>Model</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>PBCTXZ</t>
+  </si>
+  <si>
+    <t>A1C2A002PABC</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1364,6 +1367,23 @@
       </c>
       <c r="E34" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1895</v>
+      </c>
+      <c r="D35">
+        <v>5.6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated a couple little things
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="98">
   <si>
     <t>Model</t>
   </si>
@@ -181,6 +181,135 @@
   </si>
   <si>
     <t>PBCTXZ</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>ModificationID</t>
+  </si>
+  <si>
+    <t>RequestDate</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Sender</t>
+  </si>
+  <si>
+    <t>IsOption</t>
+  </si>
+  <si>
+    <t>IsNew</t>
+  </si>
+  <si>
+    <t>NewBoxSize</t>
+  </si>
+  <si>
+    <t>NewBase</t>
+  </si>
+  <si>
+    <t>NewDriveTime</t>
+  </si>
+  <si>
+    <t>NewAVTime</t>
+  </si>
+  <si>
+    <t>NewTime</t>
+  </si>
+  <si>
+    <t>NewName</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>B1C1A001</t>
+  </si>
+  <si>
+    <t>A1C3B022</t>
+  </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>B1C1A002</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>B1B1A002</t>
+  </si>
+  <si>
+    <t>Renaming model</t>
+  </si>
+  <si>
+    <t>update just drive time</t>
+  </si>
+  <si>
+    <t>update just av time</t>
+  </si>
+  <si>
+    <t>update both model times</t>
+  </si>
+  <si>
+    <t>Create new model</t>
+  </si>
+  <si>
+    <t>Rename option</t>
+  </si>
+  <si>
+    <t>update option time</t>
+  </si>
+  <si>
+    <t>Create new option</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>Update model</t>
+  </si>
+  <si>
+    <t>Update option</t>
+  </si>
+  <si>
+    <t>NewOptionCode</t>
+  </si>
+  <si>
+    <t>TU-W2</t>
+  </si>
+  <si>
+    <t>OldModelDriveTime</t>
+  </si>
+  <si>
+    <t>OldModelAVTime</t>
+  </si>
+  <si>
+    <t>OldModelBase</t>
+  </si>
+  <si>
+    <t>OldOptionCode</t>
+  </si>
+  <si>
+    <t>OIdOptionTime</t>
+  </si>
+  <si>
+    <t>OldOptionName</t>
+  </si>
+  <si>
+    <t>B1C1A003</t>
   </si>
 </sst>
 </file>
@@ -249,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -261,6 +390,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -902,6 +1039,18 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
       <c r="F10">
         <v>9001</v>
       </c>
@@ -928,6 +1077,18 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
       <c r="F11">
         <v>9002</v>
       </c>
@@ -951,6 +1112,20 @@
       </c>
       <c r="N11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -960,6 +1135,9 @@
       <c r="F14" t="s">
         <v>40</v>
       </c>
+      <c r="J14" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -983,6 +1161,18 @@
       <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1006,8 +1196,20 @@
       <c r="H16" s="7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16">
+        <v>2424</v>
+      </c>
+      <c r="L16">
+        <v>24</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1029,8 +1231,20 @@
       <c r="H17" s="7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>4848</v>
+      </c>
+      <c r="L17">
+        <v>48.6</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1052,8 +1266,20 @@
       <c r="H18" s="7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18">
+        <v>111222</v>
+      </c>
+      <c r="L18">
+        <v>28.5</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1076,7 +1302,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1099,7 +1325,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1122,7 +1348,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1145,7 +1371,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1394,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1210,7 +1436,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1224,65 +1450,870 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P29" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="S29" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U29" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="T30" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="R31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="S31" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="T31" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="V31" s="11"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13">
+        <v>43252</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12">
+        <v>0</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T32" s="12">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>55</v>
+      </c>
+      <c r="W32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13">
+        <v>43253</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32">
-        <v>2424</v>
-      </c>
-      <c r="C32">
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12">
+        <v>0</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T33" s="12">
+        <v>0</v>
+      </c>
+      <c r="U33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="W33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13">
+        <v>43254</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34" s="12">
+        <v>0</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0</v>
+      </c>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="W34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="13">
+        <v>43255</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K35" s="12">
+        <v>0</v>
+      </c>
+      <c r="L35" s="12">
+        <v>0</v>
+      </c>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T35" s="12">
+        <v>0</v>
+      </c>
+      <c r="U35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="W35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="13">
+        <v>43252</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" s="12">
+        <v>0</v>
+      </c>
+      <c r="L37" s="12">
+        <v>0</v>
+      </c>
+      <c r="M37" s="12">
+        <v>0</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P37" s="12">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="12">
+        <v>2</v>
+      </c>
+      <c r="R37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T37" s="12">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>55</v>
+      </c>
+      <c r="W37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13">
+        <v>43252</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
+      <c r="M38" s="12">
+        <v>0</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="P38" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q38" s="12">
+        <v>5</v>
+      </c>
+      <c r="R38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T38" s="12">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>55</v>
+      </c>
+      <c r="W38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="13">
+        <v>43252</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K39" s="12">
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="M39" s="12">
+        <v>0</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P39" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="12">
+        <v>5</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T39" s="12">
+        <v>0</v>
+      </c>
+      <c r="U39" t="s">
+        <v>55</v>
+      </c>
+      <c r="W39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13">
+        <v>43252</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K40" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="L40" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="M40" s="12">
+        <v>0</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="P40" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="12">
+        <v>6</v>
+      </c>
+      <c r="R40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T40" s="12">
+        <v>0</v>
+      </c>
+      <c r="U40" t="s">
+        <v>55</v>
+      </c>
+      <c r="W40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13">
+        <v>43253</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K41" s="12">
+        <v>13</v>
+      </c>
+      <c r="L41" s="12">
+        <v>1</v>
+      </c>
+      <c r="M41" s="12">
+        <v>0</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T41" s="12">
+        <v>0</v>
+      </c>
+      <c r="U41" t="s">
+        <v>55</v>
+      </c>
+      <c r="W41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="13">
+        <v>43254</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K42" s="12">
+        <v>0</v>
+      </c>
+      <c r="L42" s="12">
+        <v>0</v>
+      </c>
+      <c r="M42" s="12">
+        <v>0</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R42" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S42" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33">
-        <v>4848</v>
-      </c>
-      <c r="C33">
-        <v>48.6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34">
-        <v>111222</v>
-      </c>
-      <c r="C34">
-        <v>28.5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>14</v>
+      <c r="T42" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="U42" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="W42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="13">
+        <v>43254</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K43" s="12">
+        <v>0</v>
+      </c>
+      <c r="L43" s="12">
+        <v>0</v>
+      </c>
+      <c r="M43" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="S43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T43" s="12">
+        <v>1</v>
+      </c>
+      <c r="U43" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="13">
+        <v>43255</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K44" s="12">
+        <v>0</v>
+      </c>
+      <c r="L44" s="12">
+        <v>0</v>
+      </c>
+      <c r="M44" s="12">
+        <v>2</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R44" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="S44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T44" s="12">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
+        <v>55</v>
+      </c>
+      <c r="W44" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Supervisor table and other little things
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Option" sheetId="3" r:id="rId3"/>
+    <sheet name="TimeTrial" sheetId="4" r:id="rId4"/>
+    <sheet name="TimeTrialsOptionTime" sheetId="5" r:id="rId5"/>
+    <sheet name="Override" sheetId="6" r:id="rId6"/>
+    <sheet name="OverrideRequest" sheetId="7" r:id="rId7"/>
+    <sheet name="Modification" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="133">
   <si>
     <t>Model</t>
   </si>
@@ -186,9 +191,6 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>AT</t>
-  </si>
-  <si>
     <t>ModificationID</t>
   </si>
   <si>
@@ -213,12 +215,6 @@
     <t>IsNew</t>
   </si>
   <si>
-    <t>NewBoxSize</t>
-  </si>
-  <si>
-    <t>NewBase</t>
-  </si>
-  <si>
     <t>NewDriveTime</t>
   </si>
   <si>
@@ -267,15 +263,6 @@
     <t>TU</t>
   </si>
   <si>
-    <t>Update model</t>
-  </si>
-  <si>
-    <t>Update option</t>
-  </si>
-  <si>
-    <t>NewOptionCode</t>
-  </si>
-  <si>
     <t>TU-W2</t>
   </si>
   <si>
@@ -285,12 +272,6 @@
     <t>OldModelAVTime</t>
   </si>
   <si>
-    <t>OldModelBase</t>
-  </si>
-  <si>
-    <t>OldOptionCode</t>
-  </si>
-  <si>
     <t>OIdOptionTime</t>
   </si>
   <si>
@@ -424,6 +405,21 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>OldModel DriveTime</t>
+  </si>
+  <si>
+    <t>OldModel AVTime</t>
+  </si>
+  <si>
+    <t>OIdOption Time</t>
+  </si>
+  <si>
+    <t>OldOption Name</t>
+  </si>
+  <si>
+    <t>PABT</t>
   </si>
 </sst>
 </file>
@@ -492,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -514,6 +510,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,9 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1159,7 +1165,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1197,7 +1203,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1571,81 +1577,81 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M29" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="O29" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N30" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="Q30" s="11"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="F31" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="H31" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="I31" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="J31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L31" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="M31" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="N31" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="P31" s="11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="Q31" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="R31" s="11" t="s">
         <v>3</v>
       </c>
       <c r="S31" s="11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="T31" s="11" t="s">
         <v>16</v>
@@ -1657,7 +1663,7 @@
         <v>43253</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D32" s="12">
         <v>0</v>
@@ -1666,7 +1672,7 @@
         <v>55</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G32" s="12" t="b">
         <v>0</v>
@@ -1705,13 +1711,13 @@
         <v>6</v>
       </c>
       <c r="S32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T32" s="12" t="s">
         <v>55</v>
       </c>
       <c r="V32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -1720,7 +1726,7 @@
         <v>43255</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D33" s="12">
         <v>0</v>
@@ -1729,7 +1735,7 @@
         <v>55</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G33" s="12" t="b">
         <v>0</v>
@@ -1768,13 +1774,13 @@
         <v>6</v>
       </c>
       <c r="S33" t="s">
+        <v>71</v>
+      </c>
+      <c r="T33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V33" t="s">
         <v>74</v>
-      </c>
-      <c r="T33" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -1783,7 +1789,7 @@
         <v>43254</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D34" s="12">
         <v>0</v>
@@ -1792,7 +1798,7 @@
         <v>55</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G34" s="12" t="b">
         <v>0</v>
@@ -1831,13 +1837,13 @@
         <v>6</v>
       </c>
       <c r="S34" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="T34" s="12" t="s">
         <v>55</v>
       </c>
       <c r="V34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -1846,7 +1852,7 @@
         <v>43259</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D35" s="12">
         <v>0</v>
@@ -1855,7 +1861,7 @@
         <v>55</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G35" s="12" t="b">
         <v>0</v>
@@ -1891,16 +1897,16 @@
         <v>1</v>
       </c>
       <c r="R35" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S35" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T35" s="12" t="s">
         <v>55</v>
       </c>
       <c r="V35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -1909,7 +1915,7 @@
         <v>43257</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D36" s="12">
         <v>0</v>
@@ -1918,7 +1924,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G36" s="12" t="b">
         <v>1</v>
@@ -1954,16 +1960,16 @@
         <v>1</v>
       </c>
       <c r="R36" s="12" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="S36" s="12" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="T36" s="12" t="s">
         <v>22</v>
       </c>
       <c r="V36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -1972,7 +1978,7 @@
         <v>43260</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D37" s="12">
         <v>0</v>
@@ -1981,7 +1987,7 @@
         <v>55</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G37" s="12" t="b">
         <v>1</v>
@@ -1999,7 +2005,7 @@
         <v>2</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="M37" s="12" t="s">
         <v>55</v>
@@ -2020,13 +2026,13 @@
         <v>8</v>
       </c>
       <c r="S37" s="12" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="V37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -2035,7 +2041,7 @@
         <v>43262</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D38" s="12">
         <v>0</v>
@@ -2044,7 +2050,7 @@
         <v>55</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G38" s="12" t="b">
         <v>0</v>
@@ -2089,7 +2095,7 @@
         <v>55</v>
       </c>
       <c r="V38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -2098,7 +2104,7 @@
         <v>43263</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D39" s="12">
         <v>0</v>
@@ -2107,7 +2113,7 @@
         <v>55</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G39" s="12" t="b">
         <v>0</v>
@@ -2152,7 +2158,7 @@
         <v>55</v>
       </c>
       <c r="V39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -2161,7 +2167,7 @@
         <v>43264</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D40" s="12">
         <v>0</v>
@@ -2170,7 +2176,7 @@
         <v>55</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G40" s="12" t="b">
         <v>0</v>
@@ -2215,7 +2221,7 @@
         <v>55</v>
       </c>
       <c r="V40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -2224,7 +2230,7 @@
         <v>43265</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D41" s="12">
         <v>0</v>
@@ -2233,7 +2239,7 @@
         <v>55</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G41" s="12" t="b">
         <v>0</v>
@@ -2269,16 +2275,16 @@
         <v>1</v>
       </c>
       <c r="R41" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S41" s="12" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="T41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="V41" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -2287,7 +2293,7 @@
         <v>43267</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D42" s="12">
         <v>0</v>
@@ -2296,7 +2302,7 @@
         <v>55</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G42" s="12" t="b">
         <v>1</v>
@@ -2341,7 +2347,7 @@
         <v>20</v>
       </c>
       <c r="V42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -2350,7 +2356,7 @@
         <v>43268</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D43" s="12">
         <v>0</v>
@@ -2359,7 +2365,7 @@
         <v>55</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G43" s="12" t="b">
         <v>1</v>
@@ -2377,7 +2383,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="M43" s="12" t="s">
         <v>55</v>
@@ -2401,35 +2407,35 @@
         <v>55</v>
       </c>
       <c r="T43" s="12" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="V43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>1</v>
@@ -2441,13 +2447,13 @@
         <v>43</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -2458,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>55</v>
@@ -2490,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F48" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G48" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H48">
         <v>6</v>
@@ -2522,13 +2528,13 @@
         <v>0</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G49" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H49">
         <v>7</v>
@@ -2554,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G50" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H50">
         <v>9</v>
@@ -2586,13 +2592,13 @@
         <v>0</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G51" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H51">
         <v>8</v>
@@ -2618,13 +2624,13 @@
         <v>0</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G52" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H52">
         <v>6</v>
@@ -2650,13 +2656,13 @@
         <v>0</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G53" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H53">
         <v>6</v>
@@ -2682,13 +2688,13 @@
         <v>0</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G54" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H54">
         <v>7</v>
@@ -2714,13 +2720,13 @@
         <v>0</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G55" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H55">
         <v>7</v>
@@ -2746,13 +2752,13 @@
         <v>0</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G56" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H56">
         <v>8</v>
@@ -2778,13 +2784,13 @@
         <v>0</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G57" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H57">
         <v>7</v>
@@ -2810,13 +2816,13 @@
         <v>0</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G58" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H58">
         <v>9</v>
@@ -2842,328 +2848,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>92</v>
-      </c>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="T1" s="11"/>
+    </row>
+    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
       <c r="V2" s="11"/>
     </row>
-    <row r="3" spans="1:23" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13">
-        <v>43252</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>55</v>
-      </c>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-      <c r="M3" s="12">
-        <v>0</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="12">
-        <v>0</v>
-      </c>
-      <c r="U3" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13">
-        <v>43253</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="12">
-        <v>0</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" s="12">
-        <v>0</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13">
-        <v>43254</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
-        <v>0</v>
-      </c>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
-      <c r="W5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13">
-        <v>43255</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12" t="b">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0</v>
-      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
-      <c r="O6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
-      <c r="S6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="12">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+    </row>
+    <row r="7" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -3181,6 +3062,62 @@
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
     </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3188,12 +3125,2207 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8001</v>
+      </c>
+      <c r="B2">
+        <v>150000</v>
+      </c>
+      <c r="C2" s="8">
+        <v>43252</v>
+      </c>
+      <c r="D2">
+        <v>6.35</v>
+      </c>
+      <c r="E2">
+        <v>2.25</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8002</v>
+      </c>
+      <c r="B3">
+        <v>150000</v>
+      </c>
+      <c r="C3" s="8">
+        <v>43253</v>
+      </c>
+      <c r="D3">
+        <v>6.25</v>
+      </c>
+      <c r="E3">
+        <v>2.1</v>
+      </c>
+      <c r="F3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8003</v>
+      </c>
+      <c r="B4">
+        <v>150000</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43254</v>
+      </c>
+      <c r="D4">
+        <v>2.9</v>
+      </c>
+      <c r="E4">
+        <v>1.9</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8004</v>
+      </c>
+      <c r="B5">
+        <v>150001</v>
+      </c>
+      <c r="C5" s="8">
+        <v>43257</v>
+      </c>
+      <c r="D5">
+        <v>3.97</v>
+      </c>
+      <c r="E5">
+        <v>1.87</v>
+      </c>
+      <c r="F5">
+        <v>0.95</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8005</v>
+      </c>
+      <c r="B6">
+        <v>150001</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43258</v>
+      </c>
+      <c r="D6">
+        <v>5.07</v>
+      </c>
+      <c r="E6">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8006</v>
+      </c>
+      <c r="B7">
+        <v>150001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43258</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8007</v>
+      </c>
+      <c r="B8">
+        <v>150002</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43259</v>
+      </c>
+      <c r="D8">
+        <v>8.65</v>
+      </c>
+      <c r="E8">
+        <v>2.25</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9001</v>
+      </c>
+      <c r="B9">
+        <v>151000</v>
+      </c>
+      <c r="C9" s="8">
+        <v>43255</v>
+      </c>
+      <c r="D9">
+        <v>3.85</v>
+      </c>
+      <c r="E9">
+        <v>2.1</v>
+      </c>
+      <c r="F9">
+        <v>1.75</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9002</v>
+      </c>
+      <c r="B10">
+        <v>151000</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43256</v>
+      </c>
+      <c r="D10">
+        <v>3.6</v>
+      </c>
+      <c r="E10">
+        <v>2.1</v>
+      </c>
+      <c r="F10">
+        <v>1.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>8010</v>
+      </c>
+      <c r="B11" s="12">
+        <v>150010</v>
+      </c>
+      <c r="C11" s="13">
+        <v>43282</v>
+      </c>
+      <c r="D11" s="12">
+        <v>5.09</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>8011</v>
+      </c>
+      <c r="B12" s="12">
+        <v>150010</v>
+      </c>
+      <c r="C12" s="13">
+        <v>43282</v>
+      </c>
+      <c r="D12" s="12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7">
+        <v>8001</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7">
+        <v>8001</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7">
+        <v>8001</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7">
+        <v>8001</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6">
+        <v>8002</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6">
+        <v>8002</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6">
+        <v>8002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6">
+        <v>8002</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="7">
+        <v>146</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7">
+        <v>146</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <v>8004</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6">
+        <v>8004</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7">
+        <v>8005</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="7">
+        <v>8005</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="6">
+        <v>8007</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6">
+        <v>8007</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="6">
+        <v>8007</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6">
+        <v>8007</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12">
+        <v>8010</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12">
+        <v>8010</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12">
+        <v>8011</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12">
+        <v>8011</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>2424</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>4848</v>
+      </c>
+      <c r="C3">
+        <v>48.6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>111222</v>
+      </c>
+      <c r="C4">
+        <v>28.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="8">
+        <v>43282</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>4.5</v>
+      </c>
+      <c r="K2">
+        <v>50104100</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>43283</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>5.25</v>
+      </c>
+      <c r="K3">
+        <v>50105000</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>43284</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>6.6</v>
+      </c>
+      <c r="K4">
+        <v>50106100</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>43285</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>8.6</v>
+      </c>
+      <c r="K5">
+        <v>50108100</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>43286</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>7.25</v>
+      </c>
+      <c r="K6">
+        <v>50107000</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>43287</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>5.5</v>
+      </c>
+      <c r="K7">
+        <v>50105100</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>43288</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>5.75</v>
+      </c>
+      <c r="K8">
+        <v>50105100</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>43289</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>6.1</v>
+      </c>
+      <c r="K9">
+        <v>50106000</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>43290</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>6.75</v>
+      </c>
+      <c r="K10">
+        <v>50106100</v>
+      </c>
+      <c r="L10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>43291</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>7.1</v>
+      </c>
+      <c r="K11">
+        <v>50107000</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>43292</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>6.25</v>
+      </c>
+      <c r="K12">
+        <v>50106000</v>
+      </c>
+      <c r="L12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>43293</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>8.85</v>
+      </c>
+      <c r="K13">
+        <v>50108100</v>
+      </c>
+      <c r="L13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="15">
+        <v>43253</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="18">
+        <v>5</v>
+      </c>
+      <c r="N2" s="18">
+        <v>5</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15">
+        <v>43255</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="18">
+        <v>5</v>
+      </c>
+      <c r="N3" s="18">
+        <v>5</v>
+      </c>
+      <c r="O3" s="12">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="15">
+        <v>43254</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="J4" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="18">
+        <v>6</v>
+      </c>
+      <c r="N4" s="18">
+        <v>6</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" t="s">
+        <v>85</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15">
+        <v>43259</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>13</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>1</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15">
+        <v>43257</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>1</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15">
+        <v>43260</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>2</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>1</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15">
+        <v>43262</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>8</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="19">
+        <v>3</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15">
+        <v>43263</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>2</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="19">
+        <v>3</v>
+      </c>
+      <c r="N9" s="19">
+        <v>1</v>
+      </c>
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>1</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15">
+        <v>43264</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>9</v>
+      </c>
+      <c r="J10" s="12">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="19">
+        <v>3</v>
+      </c>
+      <c r="N10" s="19">
+        <v>1</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15">
+        <v>43265</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12">
+        <v>14</v>
+      </c>
+      <c r="J11" s="12">
+        <v>2</v>
+      </c>
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" s="12">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
+      <c r="R11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15">
+        <v>43267</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>1</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15">
+        <v>43268</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="12">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>1</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T13" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="V13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated database methods and a couple little things
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
     <t>OldOption Name</t>
   </si>
   <si>
-    <t>PABT</t>
+    <t>PAB</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -523,6 +523,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2850,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2878,7 +2888,7 @@
       <c r="Q1" s="11"/>
       <c r="T1" s="11"/>
     </row>
-    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3328,7 +3338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4482,7 +4492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4759,65 +4771,66 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21">
         <v>43259</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="20">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="12">
+      <c r="G5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20">
         <v>13</v>
       </c>
-      <c r="J5" s="12">
-        <v>1</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="12">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>1</v>
-      </c>
-      <c r="R5" s="12" t="s">
+      <c r="J5" s="20">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>1</v>
+      </c>
+      <c r="R5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="T5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated database methods and accessing
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,16 +523,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2860,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3338,7 +3338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4492,9 +4492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4814,7 +4812,7 @@
       <c r="O5" s="20">
         <v>0</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="11" t="s">
         <v>55</v>
       </c>
       <c r="Q5" s="23">
@@ -4829,8 +4827,8 @@
       <c r="T5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6" t="s">
+      <c r="U5" s="11"/>
+      <c r="V5" s="11" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated methods to fix database method changes
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2860,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4492,7 +4492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated supervisor functionality to submit to database
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -523,6 +523,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2860,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4043,7 +4053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4492,7 +4504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V6" sqref="A6:V6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4769,62 +4783,62 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21">
+      <c r="A5" s="24"/>
+      <c r="B5" s="25">
         <v>43259</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="20">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="20" t="s">
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="20">
+      <c r="G5" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="24">
         <v>13</v>
       </c>
-      <c r="J5" s="20">
-        <v>1</v>
-      </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="20">
+      <c r="J5" s="24">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="24">
         <v>0</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="23">
-        <v>1</v>
-      </c>
-      <c r="R5" s="20" t="s">
+      <c r="Q5" s="27">
+        <v>1</v>
+      </c>
+      <c r="R5" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="T5" s="24" t="s">
         <v>55</v>
       </c>
       <c r="U5" s="11"/>
@@ -4833,65 +4847,66 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21">
         <v>43257</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="20">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12">
-        <v>0</v>
-      </c>
-      <c r="J6" s="12">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
+      <c r="G6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0</v>
+      </c>
+      <c r="J6" s="20">
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
         <v>1.6</v>
       </c>
-      <c r="L6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="12">
-        <v>1</v>
-      </c>
-      <c r="P6" s="12" t="s">
+      <c r="L6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="20">
+        <v>1</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="8">
-        <v>1</v>
-      </c>
-      <c r="R6" s="12" t="s">
+      <c r="Q6" s="23">
+        <v>1</v>
+      </c>
+      <c r="R6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="12" t="s">
+      <c r="S6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="V6" t="s">
+      <c r="U6" s="6"/>
+      <c r="V6" s="6" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented submit checked function
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,15 +13,15 @@
     <sheet name="TimeTrial" sheetId="4" r:id="rId4"/>
     <sheet name="TimeTrialsOptionTime" sheetId="5" r:id="rId5"/>
     <sheet name="Override" sheetId="6" r:id="rId6"/>
-    <sheet name="OverrideRequest" sheetId="7" r:id="rId7"/>
-    <sheet name="Modification" sheetId="8" r:id="rId8"/>
+    <sheet name="Modification" sheetId="8" r:id="rId7"/>
+    <sheet name="OverrideRequest" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="138">
   <si>
     <t>Model</t>
   </si>
@@ -420,6 +420,21 @@
   </si>
   <si>
     <t>PAB</t>
+  </si>
+  <si>
+    <t>no description entered</t>
+  </si>
+  <si>
+    <t>TEMPORARY PLACEHOLDER</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>B1C1A001PB</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -488,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -523,16 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2870,7 +2875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4051,461 +4056,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="8">
-        <v>43282</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>4.5</v>
-      </c>
-      <c r="K2">
-        <v>50104100</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
-        <v>43283</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>5.25</v>
-      </c>
-      <c r="K3">
-        <v>50105000</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
-        <v>43284</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>6.6</v>
-      </c>
-      <c r="K4">
-        <v>50106100</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
-        <v>43285</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5">
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>8.6</v>
-      </c>
-      <c r="K5">
-        <v>50108100</v>
-      </c>
-      <c r="L5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
-        <v>43286</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>7.25</v>
-      </c>
-      <c r="K6">
-        <v>50107000</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
-        <v>43287</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>5.5</v>
-      </c>
-      <c r="K7">
-        <v>50105100</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
-        <v>43288</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <v>5.75</v>
-      </c>
-      <c r="K8">
-        <v>50105100</v>
-      </c>
-      <c r="L8" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
-        <v>43289</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9">
-        <v>6.1</v>
-      </c>
-      <c r="K9">
-        <v>50106000</v>
-      </c>
-      <c r="L9" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
-        <v>43290</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10">
-        <v>7</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="J10">
-        <v>6.75</v>
-      </c>
-      <c r="K10">
-        <v>50106100</v>
-      </c>
-      <c r="L10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
-        <v>43291</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11">
-        <v>8</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>7.1</v>
-      </c>
-      <c r="K11">
-        <v>50107000</v>
-      </c>
-      <c r="L11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
-        <v>43292</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
-        <v>11</v>
-      </c>
-      <c r="J12">
-        <v>6.25</v>
-      </c>
-      <c r="K12">
-        <v>50106000</v>
-      </c>
-      <c r="L12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
-        <v>43293</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>8.85</v>
-      </c>
-      <c r="K13">
-        <v>50108100</v>
-      </c>
-      <c r="L13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V6" sqref="A6:V6"/>
+      <selection activeCell="T13" sqref="T13:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4783,62 +4337,62 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21">
         <v>43259</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="24">
-        <v>0</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="24" t="s">
+      <c r="D5" s="20">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="24">
+      <c r="G5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20">
         <v>13</v>
       </c>
-      <c r="J5" s="24">
-        <v>1</v>
-      </c>
-      <c r="K5" s="24">
-        <v>0</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="24">
+      <c r="J5" s="20">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="20">
         <v>0</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="27">
-        <v>1</v>
-      </c>
-      <c r="R5" s="24" t="s">
+      <c r="Q5" s="23">
+        <v>1</v>
+      </c>
+      <c r="R5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="24" t="s">
+      <c r="T5" s="20" t="s">
         <v>55</v>
       </c>
       <c r="U5" s="11"/>
@@ -4905,8 +4459,8 @@
       <c r="T6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6" t="s">
+      <c r="U6" s="11"/>
+      <c r="V6" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -5354,4 +4908,672 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13">
+        <v>43282</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="12">
+        <v>15</v>
+      </c>
+      <c r="I2" s="12">
+        <v>50115000</v>
+      </c>
+      <c r="J2" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="K2" s="12">
+        <v>50104100</v>
+      </c>
+      <c r="L2" s="13">
+        <v>1</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13">
+        <v>43283</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12">
+        <v>6</v>
+      </c>
+      <c r="I3" s="12">
+        <v>2</v>
+      </c>
+      <c r="J3" s="12">
+        <v>5.25</v>
+      </c>
+      <c r="K3" s="12">
+        <v>50105000</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13">
+        <v>43284</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="12">
+        <v>7</v>
+      </c>
+      <c r="I4" s="12">
+        <v>3</v>
+      </c>
+      <c r="J4" s="12">
+        <v>6.6</v>
+      </c>
+      <c r="K4" s="12">
+        <v>50106100</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13">
+        <v>43285</v>
+      </c>
+      <c r="C5" s="12">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="12">
+        <v>9</v>
+      </c>
+      <c r="I5" s="12">
+        <v>4</v>
+      </c>
+      <c r="J5" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="K5" s="12">
+        <v>50108100</v>
+      </c>
+      <c r="L5" s="13">
+        <v>1</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13">
+        <v>43286</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="12">
+        <v>8</v>
+      </c>
+      <c r="I6" s="12">
+        <v>5</v>
+      </c>
+      <c r="J6" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="K6" s="12">
+        <v>50107000</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13">
+        <v>43287</v>
+      </c>
+      <c r="C7" s="12">
+        <v>6</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="K7" s="12">
+        <v>50105100</v>
+      </c>
+      <c r="L7" s="13">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13">
+        <v>43288</v>
+      </c>
+      <c r="C8" s="12">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="12">
+        <v>6</v>
+      </c>
+      <c r="I8" s="12">
+        <v>7</v>
+      </c>
+      <c r="J8" s="12">
+        <v>5.75</v>
+      </c>
+      <c r="K8" s="12">
+        <v>50105100</v>
+      </c>
+      <c r="L8" s="13">
+        <v>1</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13">
+        <v>43289</v>
+      </c>
+      <c r="C9" s="12">
+        <v>8</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="12">
+        <v>7</v>
+      </c>
+      <c r="I9" s="12">
+        <v>8</v>
+      </c>
+      <c r="J9" s="12">
+        <v>6.1</v>
+      </c>
+      <c r="K9" s="12">
+        <v>50106000</v>
+      </c>
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13">
+        <v>43290</v>
+      </c>
+      <c r="C10" s="12">
+        <v>9</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="12">
+        <v>7</v>
+      </c>
+      <c r="I10" s="12">
+        <v>9</v>
+      </c>
+      <c r="J10" s="12">
+        <v>6.75</v>
+      </c>
+      <c r="K10" s="12">
+        <v>50106100</v>
+      </c>
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13">
+        <v>43291</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="12">
+        <v>8</v>
+      </c>
+      <c r="I11" s="12">
+        <v>10</v>
+      </c>
+      <c r="J11" s="12">
+        <v>7.1</v>
+      </c>
+      <c r="K11" s="12">
+        <v>50107000</v>
+      </c>
+      <c r="L11" s="13">
+        <v>1</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13">
+        <v>43292</v>
+      </c>
+      <c r="C12" s="12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="12">
+        <v>7</v>
+      </c>
+      <c r="I12" s="12">
+        <v>11</v>
+      </c>
+      <c r="J12" s="12">
+        <v>6.25</v>
+      </c>
+      <c r="K12" s="12">
+        <v>50106000</v>
+      </c>
+      <c r="L12" s="13">
+        <v>1</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13">
+        <v>43293</v>
+      </c>
+      <c r="C13" s="12">
+        <v>12</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="12">
+        <v>9</v>
+      </c>
+      <c r="I13" s="12">
+        <v>12</v>
+      </c>
+      <c r="J13" s="12">
+        <v>8.85</v>
+      </c>
+      <c r="K13" s="12">
+        <v>50108100</v>
+      </c>
+      <c r="L13" s="13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13">
+        <v>43308</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="12">
+        <v>12</v>
+      </c>
+      <c r="I14" s="12">
+        <v>123456</v>
+      </c>
+      <c r="J14" s="12">
+        <v>10</v>
+      </c>
+      <c r="K14" s="12">
+        <v>50110000</v>
+      </c>
+      <c r="L14" s="13">
+        <v>1</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13">
+        <v>43308</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="I15" s="12">
+        <v>123457</v>
+      </c>
+      <c r="J15" s="12">
+        <v>11.2</v>
+      </c>
+      <c r="K15" s="12">
+        <v>50111000</v>
+      </c>
+      <c r="L15" s="13">
+        <v>1</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13">
+        <v>43308</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="12">
+        <v>13</v>
+      </c>
+      <c r="I16" s="12">
+        <v>50130000</v>
+      </c>
+      <c r="J16" s="12">
+        <v>10</v>
+      </c>
+      <c r="K16" s="12">
+        <v>50110000</v>
+      </c>
+      <c r="L16" s="13">
+        <v>1</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added User login functionality
</commit_message>
<xml_diff>
--- a/RouteConfiguratorDBSchema/DBTestInfo.xlsx
+++ b/RouteConfiguratorDBSchema/DBTestInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22560" windowHeight="8235" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,52 @@
     <sheet name="Override" sheetId="6" r:id="rId6"/>
     <sheet name="Modification" sheetId="8" r:id="rId7"/>
     <sheet name="OverrideRequest" sheetId="7" r:id="rId8"/>
+    <sheet name="WireGauge" sheetId="9" r:id="rId9"/>
+    <sheet name="Component" sheetId="10" r:id="rId10"/>
+    <sheet name="Enclosure" sheetId="11" r:id="rId11"/>
+    <sheet name="EngineeredModification" sheetId="12" r:id="rId12"/>
+    <sheet name="RouteQueue" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alex Turkow</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alex Turkow:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The percent of the total time that the wire gauge is going to add to the total time</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="157">
   <si>
     <t>Model</t>
   </si>
@@ -435,13 +474,70 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Gauge</t>
+  </si>
+  <si>
+    <t>TimePercentage</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Column Names</t>
+  </si>
+  <si>
+    <t>ComponentName</t>
+  </si>
+  <si>
+    <t>EnclosureSize</t>
+  </si>
+  <si>
+    <t>EnclosureType</t>
+  </si>
+  <si>
+    <t>ReviewedDate</t>
+  </si>
+  <si>
+    <t>OldTime</t>
+  </si>
+  <si>
+    <t>NewTimePercentage</t>
+  </si>
+  <si>
+    <t>OldTimePercentage</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>ProductLine</t>
+  </si>
+  <si>
+    <t>RouteQueueID</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>ModelNumber</t>
+  </si>
+  <si>
+    <t>IsApproved</t>
+  </si>
+  <si>
+    <t>AddedDate</t>
+  </si>
+  <si>
+    <t>SubmittedDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +545,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +590,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -503,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -548,6 +663,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2871,175 +2990,334 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Q4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" t="s">
+        <v>146</v>
+      </c>
+      <c r="O4" t="s">
+        <v>138</v>
+      </c>
+      <c r="P4" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:W14"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="T1" s="11"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E6">
         <v>1.5</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>1.5</v>
-      </c>
-      <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -3057,89 +3335,181 @@
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
     </row>
-    <row r="7" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="E11">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>69</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="E12">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E13">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="D14">
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="E14">
         <v>6</v>
       </c>
     </row>
@@ -3150,197 +3520,211 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D5" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D6" s="3">
         <v>1.2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D7" s="3">
         <v>1.6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D8" s="3">
         <v>0.6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D9" s="3">
         <v>0.75</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D11" s="5">
         <v>0.75</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D12" s="5">
         <v>1.35</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D15" s="5">
         <v>1.25</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D16" s="5">
         <v>1.6</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3351,355 +3735,369 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>8001</v>
       </c>
-      <c r="B2">
+      <c r="C5">
         <v>150000</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D5" s="8">
         <v>43252</v>
       </c>
-      <c r="D2">
+      <c r="E5">
         <v>6.35</v>
       </c>
-      <c r="E2">
+      <c r="F5">
         <v>2.25</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I5" t="s">
         <v>52</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>8002</v>
       </c>
-      <c r="B3">
+      <c r="C6">
         <v>150000</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D6" s="8">
         <v>43253</v>
       </c>
-      <c r="D3">
+      <c r="E6">
         <v>6.25</v>
       </c>
-      <c r="E3">
+      <c r="F6">
         <v>2.1</v>
       </c>
-      <c r="F3">
+      <c r="G6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G3">
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>8003</v>
       </c>
-      <c r="B4">
+      <c r="C7">
         <v>150000</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D7" s="8">
         <v>43254</v>
       </c>
-      <c r="D4">
+      <c r="E7">
         <v>2.9</v>
       </c>
-      <c r="E4">
+      <c r="F7">
         <v>1.9</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>8004</v>
       </c>
-      <c r="B5">
+      <c r="C8">
         <v>150001</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D8" s="8">
         <v>43257</v>
       </c>
-      <c r="D5">
+      <c r="E8">
         <v>3.97</v>
       </c>
-      <c r="E5">
+      <c r="F8">
         <v>1.87</v>
       </c>
-      <c r="F5">
+      <c r="G8">
         <v>0.95</v>
       </c>
-      <c r="G5">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I8" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>8005</v>
       </c>
-      <c r="B6">
+      <c r="C9">
         <v>150001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="D9" s="8">
         <v>43258</v>
       </c>
-      <c r="D6">
+      <c r="E9">
         <v>5.07</v>
       </c>
-      <c r="E6">
+      <c r="F9">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F6">
+      <c r="G9">
         <v>1.0900000000000001</v>
       </c>
-      <c r="G6">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I9" t="s">
         <v>53</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>8006</v>
       </c>
-      <c r="B7">
+      <c r="C10">
         <v>150001</v>
       </c>
-      <c r="C7" s="8">
+      <c r="D10" s="8">
         <v>43258</v>
       </c>
-      <c r="D7">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>8007</v>
       </c>
-      <c r="B8">
+      <c r="C11">
         <v>150002</v>
       </c>
-      <c r="C8" s="8">
+      <c r="D11" s="8">
         <v>43259</v>
       </c>
-      <c r="D8">
+      <c r="E11">
         <v>8.65</v>
       </c>
-      <c r="E8">
+      <c r="F11">
         <v>2.25</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I11" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>9001</v>
       </c>
-      <c r="B9">
+      <c r="C12">
         <v>151000</v>
       </c>
-      <c r="C9" s="8">
+      <c r="D12" s="8">
         <v>43255</v>
       </c>
-      <c r="D9">
+      <c r="E12">
         <v>3.85</v>
       </c>
-      <c r="E9">
+      <c r="F12">
         <v>2.1</v>
       </c>
-      <c r="F9">
+      <c r="G12">
         <v>1.75</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>9002</v>
       </c>
-      <c r="B10">
+      <c r="C13">
         <v>151000</v>
       </c>
-      <c r="C10" s="8">
+      <c r="D13" s="8">
         <v>43256</v>
       </c>
-      <c r="D10">
+      <c r="E13">
         <v>3.6</v>
       </c>
-      <c r="E10">
+      <c r="F13">
         <v>2.1</v>
       </c>
-      <c r="F10">
+      <c r="G13">
         <v>1.5</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
         <v>8010</v>
       </c>
-      <c r="B11" s="12">
+      <c r="C14" s="12">
         <v>150010</v>
       </c>
-      <c r="C11" s="13">
+      <c r="D14" s="13">
         <v>43282</v>
       </c>
-      <c r="D11" s="12">
+      <c r="E14" s="12">
         <v>5.09</v>
       </c>
-      <c r="E11" s="12">
+      <c r="F14" s="12">
         <v>2.2400000000000002</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G14" s="12">
         <v>0.8</v>
       </c>
-      <c r="G11" s="12">
+      <c r="H14" s="12">
         <v>2</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I14" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="J14" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
         <v>8011</v>
       </c>
-      <c r="B12" s="12">
+      <c r="C15" s="12">
         <v>150010</v>
       </c>
-      <c r="C12" s="13">
+      <c r="D15" s="13">
         <v>43282</v>
       </c>
-      <c r="D12" s="12">
+      <c r="E15" s="12">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E12" s="12">
+      <c r="F15" s="12">
         <v>1.9</v>
       </c>
-      <c r="F12" s="12">
+      <c r="G15" s="12">
         <v>0.9</v>
       </c>
-      <c r="G12" s="12">
+      <c r="H15" s="12">
         <v>2</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I15" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="J15" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3710,267 +4108,281 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="7">
+      <c r="C5" s="7">
         <v>8001</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D5" s="7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="7">
+      <c r="C6" s="7">
         <v>8001</v>
       </c>
-      <c r="C3" s="7">
+      <c r="D6" s="7">
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="7">
+      <c r="C7" s="7">
         <v>8001</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D7" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="7">
+      <c r="C8" s="7">
         <v>8001</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D8" s="7">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6">
+      <c r="C9" s="6">
         <v>8002</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D9" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6">
+      <c r="C10" s="6">
         <v>8002</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D10" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6">
+      <c r="C11" s="6">
         <v>8002</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D11" s="6">
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6">
+      <c r="C12" s="6">
         <v>8002</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D12" s="6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7">
+      <c r="C13" s="7">
         <v>146</v>
       </c>
-      <c r="C10" s="7">
+      <c r="D13" s="7">
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7">
+      <c r="C14" s="7">
         <v>146</v>
       </c>
-      <c r="C11" s="7">
+      <c r="D14" s="7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6">
+      <c r="C15" s="6">
         <v>8004</v>
       </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6">
+      <c r="C16" s="6">
         <v>8004</v>
       </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="7">
+      <c r="C17" s="7">
         <v>8005</v>
       </c>
-      <c r="C14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="7">
+      <c r="C18" s="7">
         <v>8005</v>
       </c>
-      <c r="C15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="6">
+      <c r="C19" s="6">
         <v>8007</v>
       </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6">
+      <c r="C20" s="6">
         <v>8007</v>
       </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="6">
+      <c r="C21" s="6">
         <v>8007</v>
       </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6">
+      <c r="C22" s="6">
         <v>8007</v>
       </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="12">
+      <c r="C23" s="12">
         <v>8010</v>
       </c>
-      <c r="C20" s="12">
+      <c r="D23" s="12">
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12">
+      <c r="C24" s="12">
         <v>8010</v>
       </c>
-      <c r="C21" s="12">
+      <c r="D24" s="12">
         <v>1.3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="12">
+      <c r="C25" s="12">
         <v>8011</v>
       </c>
-      <c r="C22" s="12">
+      <c r="D25" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="12">
+      <c r="C26" s="12">
         <v>8011</v>
       </c>
-      <c r="C23" s="12">
+      <c r="D26" s="12">
         <v>1.3</v>
       </c>
     </row>
@@ -3981,71 +4393,85 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="B2">
+      <c r="C5">
         <v>2424</v>
       </c>
-      <c r="C2">
+      <c r="D5">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="C6">
         <v>4848</v>
       </c>
-      <c r="C3">
+      <c r="D6">
         <v>48.6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="B4">
+      <c r="C7">
         <v>111222</v>
       </c>
-      <c r="C4">
+      <c r="D7">
         <v>28.5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4056,850 +4482,880 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A2:X16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N4" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O4" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="Q4" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R4" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="S4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="T4" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U4" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="15">
+      <c r="V4" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="15">
         <v>43253</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="12">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="12">
+      <c r="H5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
         <v>7.5</v>
       </c>
-      <c r="J2" s="12">
-        <v>0</v>
-      </c>
-      <c r="K2" s="12">
-        <v>0</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="18">
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="18">
         <v>5</v>
       </c>
-      <c r="N2" s="18">
+      <c r="O5" s="18">
         <v>5</v>
       </c>
-      <c r="O2" s="12">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="P5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
         <v>6</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T5" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="U5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="12"/>
+      <c r="X5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="15">
         <v>43255</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12">
-        <v>0</v>
-      </c>
-      <c r="J3" s="12">
+      <c r="H6" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
         <v>2.5</v>
       </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="18">
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="18">
         <v>5</v>
       </c>
-      <c r="N3" s="18">
+      <c r="O6" s="18">
         <v>5</v>
       </c>
-      <c r="O3" s="12">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="P6" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="8">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
         <v>6</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T6" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="U6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="12"/>
+      <c r="X6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15">
         <v>43254</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="12">
+      <c r="H7" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
         <v>7.5</v>
       </c>
-      <c r="J4" s="12">
+      <c r="K7" s="12">
         <v>2.5</v>
       </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="18">
         <v>6</v>
       </c>
-      <c r="N4" s="18">
+      <c r="O7" s="18">
         <v>6</v>
       </c>
-      <c r="O4" s="12">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="8">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
         <v>6</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T7" t="s">
         <v>85</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="U7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="12"/>
+      <c r="X7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+      <c r="C8" s="21">
         <v>43259</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D8" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="20">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="20" t="s">
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="20">
+      <c r="H8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="20">
         <v>13</v>
       </c>
-      <c r="J5" s="20">
-        <v>1</v>
-      </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="20">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="23">
-        <v>1</v>
-      </c>
-      <c r="R5" s="20" t="s">
+      <c r="K8" s="20">
+        <v>1</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="R8" s="23">
+        <v>1</v>
+      </c>
+      <c r="S8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="T8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11" t="s">
+      <c r="U8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="20"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21">
         <v>43257</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="20">
-        <v>0</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="20">
-        <v>0</v>
-      </c>
-      <c r="J6" s="20">
-        <v>0</v>
-      </c>
-      <c r="K6" s="20">
+      <c r="H9" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0</v>
+      </c>
+      <c r="K9" s="20">
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
         <v>1.6</v>
       </c>
-      <c r="L6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="20">
-        <v>1</v>
-      </c>
-      <c r="P6" s="20" t="s">
+      <c r="M9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="23">
-        <v>1</v>
-      </c>
-      <c r="R6" s="20" t="s">
+      <c r="R9" s="23">
+        <v>1</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="20" t="s">
+      <c r="T9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11" t="s">
+      <c r="V9" s="20"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="15">
         <v>43260</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="12">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
+      <c r="H10" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
         <v>2</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" s="12">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>1</v>
-      </c>
-      <c r="R7" s="12" t="s">
+      <c r="N10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="8">
+        <v>1</v>
+      </c>
+      <c r="S10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="12" t="s">
+      <c r="T10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V10" s="12"/>
+      <c r="X10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="15">
         <v>43262</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
+      <c r="H11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="12">
         <v>8</v>
       </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="19">
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="19">
         <v>3</v>
       </c>
-      <c r="N8" s="19">
-        <v>1</v>
-      </c>
-      <c r="O8" s="12">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>1</v>
-      </c>
-      <c r="R8" s="12" t="s">
+      <c r="O11" s="19">
+        <v>1</v>
+      </c>
+      <c r="P11" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>55</v>
+      </c>
+      <c r="R11" s="8">
+        <v>1</v>
+      </c>
+      <c r="S11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T11" t="s">
         <v>11</v>
       </c>
-      <c r="T8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V8" t="s">
+      <c r="U11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="12"/>
+      <c r="X11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="15">
         <v>43263</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12">
-        <v>0</v>
-      </c>
-      <c r="J9" s="12">
+      <c r="H12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
         <v>2</v>
       </c>
-      <c r="K9" s="12">
-        <v>0</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="19">
         <v>3</v>
       </c>
-      <c r="N9" s="19">
-        <v>1</v>
-      </c>
-      <c r="O9" s="12">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>1</v>
-      </c>
-      <c r="R9" s="12" t="s">
+      <c r="O12" s="19">
+        <v>1</v>
+      </c>
+      <c r="P12" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R12" s="8">
+        <v>1</v>
+      </c>
+      <c r="S12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T12" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V9" t="s">
+      <c r="U12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="12"/>
+      <c r="X12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="15">
         <v>43264</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12">
+      <c r="H13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
         <v>9</v>
       </c>
-      <c r="J10" s="12">
+      <c r="K13" s="12">
         <v>3</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M10" s="19">
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="19">
         <v>3</v>
       </c>
-      <c r="N10" s="19">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>1</v>
-      </c>
-      <c r="R10" s="12" t="s">
+      <c r="O13" s="19">
+        <v>1</v>
+      </c>
+      <c r="P13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>55</v>
+      </c>
+      <c r="R13" s="8">
+        <v>1</v>
+      </c>
+      <c r="S13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T13" t="s">
         <v>11</v>
       </c>
-      <c r="T10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V10" t="s">
+      <c r="U13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" s="12"/>
+      <c r="X13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="15">
         <v>43265</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="12">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="12">
+      <c r="H14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
         <v>14</v>
       </c>
-      <c r="J11" s="12">
+      <c r="K14" s="12">
         <v>2</v>
       </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" s="12">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>1</v>
-      </c>
-      <c r="R11" s="12" t="s">
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" s="8">
+        <v>1</v>
+      </c>
+      <c r="S14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="S11" s="12" t="s">
+      <c r="T14" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="T11" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="V11" t="s">
+      <c r="U14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" s="12"/>
+      <c r="X14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="15">
         <v>43267</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D15" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
+      <c r="H15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
         <v>1.8</v>
       </c>
-      <c r="L12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" s="12">
+      <c r="M15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="12">
         <v>1.35</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="Q15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" s="8">
-        <v>1</v>
-      </c>
-      <c r="R12" s="12" t="s">
+      <c r="R15" s="8">
+        <v>1</v>
+      </c>
+      <c r="S15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T12" s="12" t="s">
+      <c r="T15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V15" s="12"/>
+      <c r="X15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="15">
         <v>43268</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="12">
-        <v>0</v>
-      </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
+      <c r="H16" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="M16" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="M13" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="O13" s="12">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>1</v>
-      </c>
-      <c r="R13" s="12" t="s">
+      <c r="N16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>55</v>
+      </c>
+      <c r="R16" s="8">
+        <v>1</v>
+      </c>
+      <c r="S16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T13" s="12" t="s">
+      <c r="T16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="U16" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V16" s="12"/>
+      <c r="X16" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4910,668 +5366,734 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A2:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13">
         <v>43282</v>
       </c>
-      <c r="C2" s="12">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="G5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="12">
+      <c r="I5" s="12">
         <v>15</v>
       </c>
-      <c r="I2" s="12">
+      <c r="J5" s="12">
         <v>50115000</v>
       </c>
-      <c r="J2" s="12">
+      <c r="K5" s="12">
         <v>4.5</v>
       </c>
-      <c r="K2" s="12">
+      <c r="L5" s="12">
         <v>50104100</v>
       </c>
-      <c r="L2" s="13">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14" t="s">
+      <c r="M5" s="13">
+        <v>1</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13">
         <v>43283</v>
       </c>
-      <c r="C3" s="12">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="G6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I6" s="12">
         <v>6</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J6" s="12">
         <v>2</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K6" s="12">
         <v>5.25</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L6" s="12">
         <v>50105000</v>
       </c>
-      <c r="L3" s="13">
-        <v>1</v>
-      </c>
-      <c r="M3" s="14" t="s">
+      <c r="M6" s="13">
+        <v>1</v>
+      </c>
+      <c r="N6" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13">
         <v>43284</v>
       </c>
-      <c r="C4" s="12">
+      <c r="D7" s="12">
         <v>3</v>
       </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="G7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="12">
+      <c r="I7" s="12">
         <v>7</v>
       </c>
-      <c r="I4" s="12">
+      <c r="J7" s="12">
         <v>3</v>
       </c>
-      <c r="J4" s="12">
+      <c r="K7" s="12">
         <v>6.6</v>
       </c>
-      <c r="K4" s="12">
+      <c r="L7" s="12">
         <v>50106100</v>
       </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="14" t="s">
+      <c r="M7" s="13">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13">
         <v>43285</v>
       </c>
-      <c r="C5" s="12">
+      <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="G8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="12">
+      <c r="I8" s="12">
         <v>9</v>
       </c>
-      <c r="I5" s="12">
+      <c r="J8" s="12">
         <v>4</v>
       </c>
-      <c r="J5" s="12">
+      <c r="K8" s="12">
         <v>8.6</v>
       </c>
-      <c r="K5" s="12">
+      <c r="L8" s="12">
         <v>50108100</v>
       </c>
-      <c r="L5" s="13">
-        <v>1</v>
-      </c>
-      <c r="M5" s="14" t="s">
+      <c r="M8" s="13">
+        <v>1</v>
+      </c>
+      <c r="N8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13">
         <v>43286</v>
       </c>
-      <c r="C6" s="12">
+      <c r="D9" s="12">
         <v>5</v>
       </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="G9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="H6" s="12">
-        <v>8</v>
-      </c>
-      <c r="I6" s="12">
-        <v>5</v>
-      </c>
-      <c r="J6" s="12">
-        <v>7.25</v>
-      </c>
-      <c r="K6" s="12">
-        <v>50107000</v>
-      </c>
-      <c r="L6" s="13">
-        <v>1</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13">
-        <v>43287</v>
-      </c>
-      <c r="C7" s="12">
-        <v>6</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="12">
-        <v>6</v>
-      </c>
-      <c r="I7" s="12">
-        <v>6</v>
-      </c>
-      <c r="J7" s="12">
-        <v>5.5</v>
-      </c>
-      <c r="K7" s="12">
-        <v>50105100</v>
-      </c>
-      <c r="L7" s="13">
-        <v>1</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13">
-        <v>43288</v>
-      </c>
-      <c r="C8" s="12">
-        <v>7</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" s="12">
-        <v>6</v>
-      </c>
-      <c r="I8" s="12">
-        <v>7</v>
-      </c>
-      <c r="J8" s="12">
-        <v>5.75</v>
-      </c>
-      <c r="K8" s="12">
-        <v>50105100</v>
-      </c>
-      <c r="L8" s="13">
-        <v>1</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13">
-        <v>43289</v>
-      </c>
-      <c r="C9" s="12">
-        <v>8</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="12">
-        <v>7</v>
       </c>
       <c r="I9" s="12">
         <v>8</v>
       </c>
       <c r="J9" s="12">
+        <v>5</v>
+      </c>
+      <c r="K9" s="12">
+        <v>7.25</v>
+      </c>
+      <c r="L9" s="12">
+        <v>50107000</v>
+      </c>
+      <c r="M9" s="13">
+        <v>1</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13">
+        <v>43287</v>
+      </c>
+      <c r="D10" s="12">
+        <v>6</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="12">
+        <v>6</v>
+      </c>
+      <c r="J10" s="12">
+        <v>6</v>
+      </c>
+      <c r="K10" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="L10" s="12">
+        <v>50105100</v>
+      </c>
+      <c r="M10" s="13">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13">
+        <v>43288</v>
+      </c>
+      <c r="D11" s="12">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="12">
+        <v>6</v>
+      </c>
+      <c r="J11" s="12">
+        <v>7</v>
+      </c>
+      <c r="K11" s="12">
+        <v>5.75</v>
+      </c>
+      <c r="L11" s="12">
+        <v>50105100</v>
+      </c>
+      <c r="M11" s="13">
+        <v>1</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13">
+        <v>43289</v>
+      </c>
+      <c r="D12" s="12">
+        <v>8</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="12">
+        <v>7</v>
+      </c>
+      <c r="J12" s="12">
+        <v>8</v>
+      </c>
+      <c r="K12" s="12">
         <v>6.1</v>
       </c>
-      <c r="K9" s="12">
+      <c r="L12" s="12">
         <v>50106000</v>
       </c>
-      <c r="L9" s="13">
-        <v>1</v>
-      </c>
-      <c r="M9" s="14" t="s">
+      <c r="M12" s="13">
+        <v>1</v>
+      </c>
+      <c r="N12" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13">
         <v>43290</v>
       </c>
-      <c r="C10" s="12">
+      <c r="D13" s="12">
         <v>9</v>
       </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="G13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="12">
+      <c r="I13" s="12">
         <v>7</v>
       </c>
-      <c r="I10" s="12">
+      <c r="J13" s="12">
         <v>9</v>
       </c>
-      <c r="J10" s="12">
+      <c r="K13" s="12">
         <v>6.75</v>
       </c>
-      <c r="K10" s="12">
+      <c r="L13" s="12">
         <v>50106100</v>
       </c>
-      <c r="L10" s="13">
-        <v>1</v>
-      </c>
-      <c r="M10" s="14" t="s">
+      <c r="M13" s="13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13">
         <v>43291</v>
       </c>
-      <c r="C11" s="12">
+      <c r="D14" s="12">
         <v>10</v>
       </c>
-      <c r="D11" s="12">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="G14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="12">
+      <c r="I14" s="12">
         <v>8</v>
-      </c>
-      <c r="I11" s="12">
-        <v>10</v>
-      </c>
-      <c r="J11" s="12">
-        <v>7.1</v>
-      </c>
-      <c r="K11" s="12">
-        <v>50107000</v>
-      </c>
-      <c r="L11" s="13">
-        <v>1</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13">
-        <v>43292</v>
-      </c>
-      <c r="C12" s="12">
-        <v>11</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" s="12">
-        <v>7</v>
-      </c>
-      <c r="I12" s="12">
-        <v>11</v>
-      </c>
-      <c r="J12" s="12">
-        <v>6.25</v>
-      </c>
-      <c r="K12" s="12">
-        <v>50106000</v>
-      </c>
-      <c r="L12" s="13">
-        <v>1</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13">
-        <v>43293</v>
-      </c>
-      <c r="C13" s="12">
-        <v>12</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" s="12">
-        <v>9</v>
-      </c>
-      <c r="I13" s="12">
-        <v>12</v>
-      </c>
-      <c r="J13" s="12">
-        <v>8.85</v>
-      </c>
-      <c r="K13" s="12">
-        <v>50108100</v>
-      </c>
-      <c r="L13" s="13">
-        <v>1</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13">
-        <v>43308</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="12">
-        <v>12</v>
-      </c>
-      <c r="I14" s="12">
-        <v>123456</v>
       </c>
       <c r="J14" s="12">
         <v>10</v>
       </c>
       <c r="K14" s="12">
+        <v>7.1</v>
+      </c>
+      <c r="L14" s="12">
+        <v>50107000</v>
+      </c>
+      <c r="M14" s="13">
+        <v>1</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13">
+        <v>43292</v>
+      </c>
+      <c r="D15" s="12">
+        <v>11</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="12">
+        <v>7</v>
+      </c>
+      <c r="J15" s="12">
+        <v>11</v>
+      </c>
+      <c r="K15" s="12">
+        <v>6.25</v>
+      </c>
+      <c r="L15" s="12">
+        <v>50106000</v>
+      </c>
+      <c r="M15" s="13">
+        <v>1</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13">
+        <v>43293</v>
+      </c>
+      <c r="D16" s="12">
+        <v>12</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="12">
+        <v>9</v>
+      </c>
+      <c r="J16" s="12">
+        <v>12</v>
+      </c>
+      <c r="K16" s="12">
+        <v>8.85</v>
+      </c>
+      <c r="L16" s="12">
+        <v>50108100</v>
+      </c>
+      <c r="M16" s="13">
+        <v>1</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13">
+        <v>43308</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="12">
+        <v>12</v>
+      </c>
+      <c r="J17" s="12">
+        <v>123456</v>
+      </c>
+      <c r="K17" s="12">
+        <v>10</v>
+      </c>
+      <c r="L17" s="12">
         <v>50110000</v>
       </c>
-      <c r="L14" s="13">
-        <v>1</v>
-      </c>
-      <c r="M14" s="12" t="s">
+      <c r="M17" s="13">
+        <v>1</v>
+      </c>
+      <c r="N17" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13">
         <v>43308</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D18" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="G18" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="H15" s="12">
+      <c r="I18" s="12">
         <v>12.5</v>
       </c>
-      <c r="I15" s="12">
+      <c r="J18" s="12">
         <v>123457</v>
       </c>
-      <c r="J15" s="12">
+      <c r="K18" s="12">
         <v>11.2</v>
       </c>
-      <c r="K15" s="12">
+      <c r="L18" s="12">
         <v>50111000</v>
       </c>
-      <c r="L15" s="13">
-        <v>1</v>
-      </c>
-      <c r="M15" s="12" t="s">
+      <c r="M18" s="13">
+        <v>1</v>
+      </c>
+      <c r="N18" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13">
         <v>43308</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D19" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12" t="s">
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="G19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="12">
+      <c r="I19" s="12">
         <v>13</v>
       </c>
-      <c r="I16" s="12">
+      <c r="J19" s="12">
         <v>50130000</v>
       </c>
-      <c r="J16" s="12">
+      <c r="K19" s="12">
         <v>10</v>
       </c>
-      <c r="K16" s="12">
+      <c r="L19" s="12">
         <v>50110000</v>
       </c>
-      <c r="L16" s="13">
-        <v>1</v>
-      </c>
-      <c r="M16" s="12" t="s">
+      <c r="M19" s="13">
+        <v>1</v>
+      </c>
+      <c r="N19" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>